<commit_message>
Fix for Newton-Raphson method
</commit_message>
<xml_diff>
--- a/Roots of Nonlinear Equations.xlsx
+++ b/Roots of Nonlinear Equations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24301"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24322"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ramiro Olivencia\WebstormProjects\matematica-superior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6C35549-DAA7-45DB-9270-EDDD38D14279}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5FB731A-ABC9-48A8-B523-D55D322F4273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17175" yWindow="3240" windowWidth="25800" windowHeight="21000" xr2:uid="{B71A5E63-7F95-49DA-9D39-46DB68373441}"/>
+    <workbookView xWindow="1170" yWindow="600" windowWidth="25800" windowHeight="21000" activeTab="2" xr2:uid="{B71A5E63-7F95-49DA-9D39-46DB68373441}"/>
   </bookViews>
   <sheets>
     <sheet name="Root Isolation" sheetId="5" r:id="rId1"/>
@@ -728,15 +728,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -755,22 +746,21 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="25" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="2"/>
@@ -778,56 +768,6 @@
       <fill>
         <patternFill>
           <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1158,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD5361A1-895A-4CBC-AA18-B4DC4767720E}">
   <dimension ref="B1:S12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N20" sqref="N20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1206,20 +1146,20 @@
       <c r="H3" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="L3" s="42"/>
-      <c r="M3" s="42"/>
-      <c r="N3" s="42"/>
-      <c r="O3" s="42"/>
-      <c r="P3" s="42" t="str">
+      <c r="L3" s="56"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="56"/>
+      <c r="O3" s="56"/>
+      <c r="P3" s="56" t="str">
         <f>_xlfn.CONCAT("Valid Interval: ", "I = [", C1, ";", E1,"]")</f>
         <v>Valid Interval: I = [-8;0]</v>
       </c>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="42"/>
-      <c r="S3" s="43"/>
+      <c r="Q3" s="56"/>
+      <c r="R3" s="56"/>
+      <c r="S3" s="57"/>
     </row>
     <row r="4" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="21">
@@ -1250,25 +1190,25 @@
       <c r="L4" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="M4" s="44">
+      <c r="M4" s="41">
         <v>-3</v>
       </c>
-      <c r="N4" s="44">
+      <c r="N4" s="41">
         <v>-2</v>
       </c>
-      <c r="O4" s="44">
+      <c r="O4" s="41">
         <v>-1</v>
       </c>
-      <c r="P4" s="44">
+      <c r="P4" s="41">
         <v>0</v>
       </c>
-      <c r="Q4" s="44">
+      <c r="Q4" s="41">
         <v>1</v>
       </c>
-      <c r="R4" s="44">
+      <c r="R4" s="41">
         <v>2</v>
       </c>
-      <c r="S4" s="45">
+      <c r="S4" s="42">
         <v>3</v>
       </c>
     </row>
@@ -1296,35 +1236,35 @@
         <f t="shared" ref="H5:H9" si="0">IF(SIGN(F5) &lt;&gt; SIGN(G5), "Yes", "No")</f>
         <v>No</v>
       </c>
-      <c r="K5" s="46">
+      <c r="K5" s="43">
         <v>-2.1351200000000001</v>
       </c>
-      <c r="L5" s="55"/>
-      <c r="M5" s="49">
-        <f t="shared" ref="L5:O8" si="1">$K$5 + 2*PI()*M4</f>
+      <c r="L5" s="52"/>
+      <c r="M5" s="46">
+        <f t="shared" ref="M5:O8" si="1">$K$5 + 2*PI()*M4</f>
         <v>-20.984675921538759</v>
       </c>
-      <c r="N5" s="49">
+      <c r="N5" s="46">
         <f t="shared" si="1"/>
         <v>-14.701490614359173</v>
       </c>
-      <c r="O5" s="49">
+      <c r="O5" s="46">
         <f t="shared" si="1"/>
         <v>-8.4183053071795868</v>
       </c>
-      <c r="P5" s="49">
+      <c r="P5" s="46">
         <f>$K$5 + 2*PI()*P4</f>
         <v>-2.1351200000000001</v>
       </c>
-      <c r="Q5" s="49">
+      <c r="Q5" s="46">
         <f t="shared" ref="Q5:S5" si="2">$K$5 + 2*PI()*Q4</f>
         <v>4.1480653071795857</v>
       </c>
-      <c r="R5" s="49">
+      <c r="R5" s="46">
         <f t="shared" si="2"/>
         <v>10.431250614359172</v>
       </c>
-      <c r="S5" s="50">
+      <c r="S5" s="47">
         <f t="shared" si="2"/>
         <v>16.714435921538758</v>
       </c>
@@ -1353,35 +1293,35 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="44">
         <v>-0.36296899999999999</v>
       </c>
-      <c r="L6" s="56"/>
-      <c r="M6" s="51">
+      <c r="L6" s="53"/>
+      <c r="M6" s="48">
         <f t="shared" si="1"/>
         <v>-133.98572742613757</v>
       </c>
-      <c r="N6" s="51">
+      <c r="N6" s="48">
         <f t="shared" si="1"/>
         <v>-94.50730982178014</v>
       </c>
-      <c r="O6" s="51">
+      <c r="O6" s="48">
         <f>$K$6 + 2*PI()*O4</f>
         <v>-6.6461543071795859</v>
       </c>
-      <c r="P6" s="51">
+      <c r="P6" s="48">
         <f>$K$6 + 2*PI()*P4</f>
         <v>-0.36296899999999999</v>
       </c>
-      <c r="Q6" s="51">
+      <c r="Q6" s="48">
         <f t="shared" ref="Q6:S6" si="3">$K$6 + 2*PI()*Q4</f>
         <v>5.9202163071795866</v>
       </c>
-      <c r="R6" s="51">
+      <c r="R6" s="48">
         <f t="shared" si="3"/>
         <v>12.203401614359173</v>
       </c>
-      <c r="S6" s="52">
+      <c r="S6" s="49">
         <f t="shared" si="3"/>
         <v>18.486586921538759</v>
       </c>
@@ -1410,35 +1350,35 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="44">
         <v>0.36296899999999999</v>
       </c>
-      <c r="L7" s="56"/>
-      <c r="M7" s="51">
+      <c r="L7" s="53"/>
+      <c r="M7" s="48">
         <f t="shared" si="1"/>
         <v>-843.99227393567651</v>
       </c>
-      <c r="N7" s="51">
+      <c r="N7" s="48">
         <f t="shared" si="1"/>
         <v>-595.94206049327795</v>
       </c>
-      <c r="O7" s="51">
+      <c r="O7" s="48">
         <f>$K$7 + 2*PI()*O4</f>
         <v>-5.9202163071795866</v>
       </c>
-      <c r="P7" s="51">
+      <c r="P7" s="48">
         <f>$K$6 + 2*PI()*P5</f>
         <v>-13.778323613065279</v>
       </c>
-      <c r="Q7" s="51">
+      <c r="Q7" s="48">
         <f t="shared" ref="Q7:S7" si="4">$K$6 + 2*PI()*Q5</f>
         <v>25.70009399129215</v>
       </c>
-      <c r="R7" s="51">
+      <c r="R7" s="48">
         <f t="shared" si="4"/>
         <v>65.178511595649567</v>
       </c>
-      <c r="S7" s="52">
+      <c r="S7" s="49">
         <f t="shared" si="4"/>
         <v>104.656929200007</v>
       </c>
@@ -1467,35 +1407,35 @@
         <f t="shared" si="0"/>
         <v>Yes</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="44">
         <v>2.1351200000000001</v>
       </c>
-      <c r="L8" s="56"/>
-      <c r="M8" s="51">
+      <c r="L8" s="53"/>
+      <c r="M8" s="48">
         <f t="shared" si="1"/>
         <v>-5305.0949749657311</v>
       </c>
-      <c r="N8" s="51">
+      <c r="N8" s="48">
         <f t="shared" si="1"/>
         <v>-3746.549518421692</v>
       </c>
-      <c r="O8" s="51">
+      <c r="O8" s="48">
         <f>$K$8 + 2*PI()*O4</f>
         <v>-4.1480653071795857</v>
       </c>
-      <c r="P8" s="51">
+      <c r="P8" s="48">
         <f>$K$6 + 2*PI()*P6</f>
         <v>-2.643570487761667</v>
       </c>
-      <c r="Q8" s="51">
+      <c r="Q8" s="48">
         <f t="shared" ref="Q8:S8" si="5">$K$6 + 2*PI()*Q6</f>
         <v>36.834847116595768</v>
       </c>
-      <c r="R8" s="51">
+      <c r="R8" s="48">
         <f t="shared" si="5"/>
         <v>76.313264720953185</v>
       </c>
-      <c r="S8" s="52">
+      <c r="S8" s="49">
         <f t="shared" si="5"/>
         <v>115.79168232531062</v>
       </c>
@@ -1524,48 +1464,48 @@
         <f t="shared" si="0"/>
         <v>No</v>
       </c>
-      <c r="K9" s="47"/>
-      <c r="L9" s="56"/>
-      <c r="M9" s="51"/>
-      <c r="N9" s="51"/>
-      <c r="O9" s="51"/>
-      <c r="P9" s="51"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="51"/>
-      <c r="S9" s="52"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="53"/>
+      <c r="M9" s="48"/>
+      <c r="N9" s="48"/>
+      <c r="O9" s="48"/>
+      <c r="P9" s="48"/>
+      <c r="Q9" s="48"/>
+      <c r="R9" s="48"/>
+      <c r="S9" s="49"/>
     </row>
     <row r="10" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K10" s="47"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="51"/>
-      <c r="N10" s="51"/>
-      <c r="O10" s="51"/>
-      <c r="P10" s="51"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="51"/>
-      <c r="S10" s="52"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="53"/>
+      <c r="M10" s="48"/>
+      <c r="N10" s="48"/>
+      <c r="O10" s="48"/>
+      <c r="P10" s="48"/>
+      <c r="Q10" s="48"/>
+      <c r="R10" s="48"/>
+      <c r="S10" s="49"/>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="K11" s="47"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="51"/>
-      <c r="N11" s="51"/>
-      <c r="O11" s="51"/>
-      <c r="P11" s="51"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="51"/>
-      <c r="S11" s="52"/>
+      <c r="K11" s="44"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="48"/>
+      <c r="N11" s="48"/>
+      <c r="O11" s="48"/>
+      <c r="P11" s="48"/>
+      <c r="Q11" s="48"/>
+      <c r="R11" s="48"/>
+      <c r="S11" s="49"/>
     </row>
     <row r="12" spans="2:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="K12" s="48"/>
-      <c r="L12" s="57"/>
-      <c r="M12" s="53"/>
-      <c r="N12" s="53"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="53"/>
-      <c r="Q12" s="53"/>
-      <c r="R12" s="53"/>
-      <c r="S12" s="54"/>
+      <c r="K12" s="45"/>
+      <c r="L12" s="54"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="50"/>
+      <c r="Q12" s="50"/>
+      <c r="R12" s="50"/>
+      <c r="S12" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1573,11 +1513,11 @@
     <mergeCell ref="P3:S3"/>
   </mergeCells>
   <conditionalFormatting sqref="M5:S12">
-    <cfRule type="cellIs" dxfId="2" priority="6" operator="notBetween">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="notBetween">
       <formula>$C$1</formula>
       <formula>$E$1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>$C$1</formula>
       <formula>$E$1</formula>
     </cfRule>
@@ -1829,7 +1769,7 @@
         <v>-9.753461088571615E-3</v>
       </c>
       <c r="I6" s="10">
-        <f t="shared" ref="I4:I11" si="4">ABS((E6-E5)/E6)</f>
+        <f t="shared" ref="I6:I11" si="4">ABS((E6-E5)/E6)</f>
         <v>2.8459412054331989E-4</v>
       </c>
       <c r="J6" s="10" cm="1">
@@ -2077,7 +2017,7 @@
         <v>6.2420221480821714E-2</v>
       </c>
       <c r="D12" s="6">
-        <f t="shared" ref="D12:D46" si="5">D11+1</f>
+        <f t="shared" ref="D12:D22" si="5">D11+1</f>
         <v>10</v>
       </c>
       <c r="E12" s="10">
@@ -2504,13 +2444,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF2ECEA1-6647-455D-AA68-E94BA6B65565}">
   <dimension ref="B1:L22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
     <col min="5" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
@@ -2618,15 +2559,15 @@
       </c>
       <c r="J3" s="10" cm="1">
         <f t="array" ref="J3">ABS(f_x(E3))/ABS($C$8)</f>
-        <v>2.161581858995399E-2</v>
+        <v>50038.772370039791</v>
       </c>
       <c r="K3" s="10" cm="1">
         <f t="array" ref="K3">E3 - ABS(f_x(E3))/ABS($C$8)</f>
-        <v>-7.3043960558927212</v>
+        <v>-50046.05515027709</v>
       </c>
       <c r="L3" s="10" cm="1">
         <f t="array" ref="L3">E3 + ABS(f_x(E3))/ABS($C$8)</f>
-        <v>-7.2611644187128137</v>
+        <v>50031.489589802492</v>
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
@@ -2663,15 +2604,15 @@
       </c>
       <c r="J4" s="10" cm="1">
         <f t="array" ref="J4">ABS(f_x(E4))/ABS($C$8)</f>
-        <v>3.1736189615194914E-4</v>
+        <v>734.66566229659452</v>
       </c>
       <c r="K4" s="10" cm="1">
         <f t="array" ref="K4">E4 - ABS(f_x(E4))/ABS($C$8)</f>
-        <v>-7.2616516910079092</v>
+        <v>-741.92699662570624</v>
       </c>
       <c r="L4" s="10" cm="1">
         <f t="array" ref="L4">E4 + ABS(f_x(E4))/ABS($C$8)</f>
-        <v>-7.2610169672156051</v>
+        <v>727.4043279674828</v>
       </c>
     </row>
     <row r="5" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2708,15 +2649,15 @@
       </c>
       <c r="J5" s="10" cm="1">
         <f t="array" ref="J5">ABS(f_x(E5))/ABS($C$8)</f>
-        <v>7.4445986256183506E-8</v>
+        <v>0.17233609472775491</v>
       </c>
       <c r="K5" s="10" cm="1">
         <f t="array" ref="K5">E5 - ABS(f_x(E5))/ABS($C$8)</f>
-        <v>-7.26100994972471</v>
+        <v>-7.4333459700064788</v>
       </c>
       <c r="L5" s="10" cm="1">
         <f t="array" ref="L5">E5 + ABS(f_x(E5))/ABS($C$8)</f>
-        <v>-7.2610098008327375</v>
+        <v>-7.0886737805509688</v>
       </c>
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
@@ -2753,15 +2694,15 @@
       </c>
       <c r="J6" s="10" cm="1">
         <f t="array" ref="J6">ABS(f_x(E6))/ABS($C$8)</f>
-        <v>4.0251318566684846E-15</v>
+        <v>9.3178361900593009E-9</v>
       </c>
       <c r="K6" s="10" cm="1">
         <f t="array" ref="K6">E6 - ABS(f_x(E6))/ABS($C$8)</f>
-        <v>-7.2610097991334053</v>
+        <v>-7.2610098084512371</v>
       </c>
       <c r="L6" s="10" cm="1">
         <f t="array" ref="L6">E6 + ABS(f_x(E6))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097898155646</v>
       </c>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
@@ -2798,15 +2739,15 @@
       </c>
       <c r="J7" s="10" cm="1">
         <f t="array" ref="J7">ABS(f_x(E7))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K7" s="10" cm="1">
         <f t="array" ref="K7">E7 - ABS(f_x(E7))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L7" s="10" cm="1">
         <f t="array" ref="L7">E7 + ABS(f_x(E7))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="8" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2814,8 +2755,8 @@
         <v>17</v>
       </c>
       <c r="C8" s="16">
-        <f>MIN(C6,C7)</f>
-        <v>-0.42062972663824688</v>
+        <f>MIN(ABS(C6),ABS(C7))</f>
+        <v>1.8170421522967217E-7</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="1"/>
@@ -2843,15 +2784,15 @@
       </c>
       <c r="J8" s="10" cm="1">
         <f t="array" ref="J8">ABS(f_x(E8))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K8" s="10" cm="1">
         <f t="array" ref="K8">E8 - ABS(f_x(E8))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L8" s="10" cm="1">
         <f t="array" ref="L8">E8 + ABS(f_x(E8))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -2887,15 +2828,15 @@
       </c>
       <c r="J9" s="10" cm="1">
         <f t="array" ref="J9">ABS(f_x(E9))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K9" s="10" cm="1">
         <f t="array" ref="K9">E9 - ABS(f_x(E9))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L9" s="10" cm="1">
         <f t="array" ref="L9">E9 + ABS(f_x(E9))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2932,15 +2873,15 @@
       </c>
       <c r="J10" s="10" cm="1">
         <f t="array" ref="J10">ABS(f_x(E10))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K10" s="10" cm="1">
         <f t="array" ref="K10">E10 - ABS(f_x(E10))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L10" s="10" cm="1">
         <f t="array" ref="L10">E10 + ABS(f_x(E10))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
@@ -2970,15 +2911,15 @@
       </c>
       <c r="J11" s="10" cm="1">
         <f t="array" ref="J11">ABS(f_x(E11))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K11" s="10" cm="1">
         <f t="array" ref="K11">E11 - ABS(f_x(E11))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L11" s="10" cm="1">
         <f t="array" ref="L11">E11 + ABS(f_x(E11))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
@@ -3008,15 +2949,15 @@
       </c>
       <c r="J12" s="10" cm="1">
         <f t="array" ref="J12">ABS(f_x(E12))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K12" s="10" cm="1">
         <f t="array" ref="K12">E12 - ABS(f_x(E12))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L12" s="10" cm="1">
         <f t="array" ref="L12">E12 + ABS(f_x(E12))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -3046,15 +2987,15 @@
       </c>
       <c r="J13" s="10" cm="1">
         <f t="array" ref="J13">ABS(f_x(E13))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K13" s="10" cm="1">
         <f t="array" ref="K13">E13 - ABS(f_x(E13))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L13" s="10" cm="1">
         <f t="array" ref="L13">E13 + ABS(f_x(E13))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
@@ -3084,15 +3025,15 @@
       </c>
       <c r="J14" s="10" cm="1">
         <f t="array" ref="J14">ABS(f_x(E14))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K14" s="10" cm="1">
         <f t="array" ref="K14">E14 - ABS(f_x(E14))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L14" s="10" cm="1">
         <f t="array" ref="L14">E14 + ABS(f_x(E14))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
@@ -3122,15 +3063,15 @@
       </c>
       <c r="J15" s="10" cm="1">
         <f t="array" ref="J15">ABS(f_x(E15))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K15" s="10" cm="1">
         <f t="array" ref="K15">E15 - ABS(f_x(E15))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L15" s="10" cm="1">
         <f t="array" ref="L15">E15 + ABS(f_x(E15))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
@@ -3160,15 +3101,15 @@
       </c>
       <c r="J16" s="10" cm="1">
         <f t="array" ref="J16">ABS(f_x(E16))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K16" s="10" cm="1">
         <f t="array" ref="K16">E16 - ABS(f_x(E16))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L16" s="10" cm="1">
         <f t="array" ref="L16">E16 + ABS(f_x(E16))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="17" spans="4:12" x14ac:dyDescent="0.25">
@@ -3198,15 +3139,15 @@
       </c>
       <c r="J17" s="10" cm="1">
         <f t="array" ref="J17">ABS(f_x(E17))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K17" s="10" cm="1">
         <f t="array" ref="K17">E17 - ABS(f_x(E17))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L17" s="10" cm="1">
         <f t="array" ref="L17">E17 + ABS(f_x(E17))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="18" spans="4:12" x14ac:dyDescent="0.25">
@@ -3236,15 +3177,15 @@
       </c>
       <c r="J18" s="10" cm="1">
         <f t="array" ref="J18">ABS(f_x(E18))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K18" s="10" cm="1">
         <f t="array" ref="K18">E18 - ABS(f_x(E18))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L18" s="10" cm="1">
         <f t="array" ref="L18">E18 + ABS(f_x(E18))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="19" spans="4:12" x14ac:dyDescent="0.25">
@@ -3274,15 +3215,15 @@
       </c>
       <c r="J19" s="10" cm="1">
         <f t="array" ref="J19">ABS(f_x(E19))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K19" s="10" cm="1">
         <f t="array" ref="K19">E19 - ABS(f_x(E19))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L19" s="10" cm="1">
         <f t="array" ref="L19">E19 + ABS(f_x(E19))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="20" spans="4:12" x14ac:dyDescent="0.25">
@@ -3312,15 +3253,15 @@
       </c>
       <c r="J20" s="10" cm="1">
         <f t="array" ref="J20">ABS(f_x(E20))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K20" s="10" cm="1">
         <f t="array" ref="K20">E20 - ABS(f_x(E20))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L20" s="10" cm="1">
         <f t="array" ref="L20">E20 + ABS(f_x(E20))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="21" spans="4:12" x14ac:dyDescent="0.25">
@@ -3350,15 +3291,15 @@
       </c>
       <c r="J21" s="10" cm="1">
         <f t="array" ref="J21">ABS(f_x(E21))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K21" s="10" cm="1">
         <f t="array" ref="K21">E21 - ABS(f_x(E21))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L21" s="10" cm="1">
         <f t="array" ref="L21">E21 + ABS(f_x(E21))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
     <row r="22" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3388,15 +3329,15 @@
       </c>
       <c r="J22" s="11" cm="1">
         <f t="array" ref="J22">ABS(f_x(E22))/ABS($C$8)</f>
-        <v>2.639430725684252E-16</v>
+        <v>6.1100565180716723E-10</v>
       </c>
       <c r="K22" s="11" cm="1">
         <f t="array" ref="K22">E22 - ABS(f_x(E22))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097997444019</v>
       </c>
       <c r="L22" s="11" cm="1">
         <f t="array" ref="L22">E22 + ABS(f_x(E22))/ABS($C$8)</f>
-        <v>-7.2610097991333964</v>
+        <v>-7.2610097985223909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>